<commit_message>
hoan thanh data user
</commit_message>
<xml_diff>
--- a/data/company.xlsx
+++ b/data/company.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1095B71-0CD8-4982-B3CE-ECB1FDCC4046}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6896781-BD98-4E21-B742-3996BFE63AF7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8925" yWindow="240" windowWidth="17670" windowHeight="14985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>name</t>
   </si>
@@ -34,21 +34,23 @@
     <t>SBA</t>
   </si>
   <si>
-    <t>ABC</t>
-  </si>
-  <si>
     <t>isActive</t>
-  </si>
-  <si>
-    <t>Công ty cổ phần ABC</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -76,8 +78,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -358,10 +361,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A3" sqref="A3:C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -371,14 +374,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>5</v>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -389,17 +392,6 @@
         <v>3</v>
       </c>
       <c r="C2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3">
         <v>1</v>
       </c>
     </row>

</xml_diff>